<commit_message>
DONE (most of what I can at least) if i have to find more coordinates ill kill someone
</commit_message>
<xml_diff>
--- a/CurrentMrktsCounty.xlsx
+++ b/CurrentMrktsCounty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chesneymelissinos/Desktop/Coding/lafpc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6054D3-803D-6D46-88ED-E12289D1BBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706AC4C0-B089-844E-B3B6-0EE524CAAA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="500" windowWidth="20380" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2320" yWindow="500" windowWidth="26480" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -5277,25 +5277,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">470 Hawaiian Ave., Providence Wellmess
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Center, Wilmington, 90744</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>Nancy Ramos</t>
     </r>
   </si>
@@ -7432,6 +7413,10 @@
   <si>
     <t>7248 Owensmouth Ave. between Wyandotte St. &amp; Sherman Wy., Canoga
 Park, 91303</t>
+  </si>
+  <si>
+    <t>470 Hawaiian Ave., Providence Wellness
+Center, Wilmington, 90744</t>
   </si>
 </sst>
 </file>
@@ -7498,7 +7483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -7527,15 +7512,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7887,8 +7863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7928,10 +7904,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7961,28 +7937,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -8018,35 +7994,35 @@
         <v>-118.38246917724599</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5">
         <v>34.182926177978501</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5">
         <v>-118.30867767333901</v>
       </c>
     </row>
@@ -8199,25 +8175,25 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="8"/>
@@ -8691,28 +8667,28 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="10" t="s">
         <v>157</v>
       </c>
     </row>
@@ -9020,31 +8996,31 @@
       <c r="G37" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="15"/>
+      <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="10" t="s">
         <v>115</v>
       </c>
     </row>
@@ -9145,28 +9121,28 @@
       </c>
     </row>
     <row r="42" spans="1:10" s="9" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="13" t="s">
+      <c r="A42" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>208</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="10" t="s">
         <v>211</v>
       </c>
     </row>
@@ -9235,28 +9211,28 @@
       </c>
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="13" t="s">
+      <c r="A45" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="13" t="s">
+      <c r="H45" s="10" t="s">
         <v>223</v>
       </c>
     </row>
@@ -9646,7 +9622,7 @@
         <v>270</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>271</v>
@@ -10043,28 +10019,28 @@
       </c>
     </row>
     <row r="71" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B71" s="14" t="s">
+      <c r="A71" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" s="11" t="s">
         <v>314</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="E71" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="G71" s="14" t="s">
+      <c r="G71" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H71" s="13" t="s">
+      <c r="H71" s="10" t="s">
         <v>317</v>
       </c>
     </row>
@@ -10536,29 +10512,29 @@
         <v>-118.3910673</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B87" s="3" t="s">
+    <row r="87" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E87" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F87" s="3" t="s">
+      <c r="F87" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="G87" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H87" s="3" t="s">
+      <c r="H87" s="7" t="s">
         <v>368</v>
       </c>
     </row>
@@ -10587,6 +10563,12 @@
       <c r="H88" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="I88">
+        <v>33.958495999999997</v>
+      </c>
+      <c r="J88">
+        <v>-118.39367</v>
+      </c>
     </row>
     <row r="89" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
@@ -10613,6 +10595,12 @@
       <c r="H89" s="4" t="s">
         <v>311</v>
       </c>
+      <c r="I89">
+        <v>34.1015278</v>
+      </c>
+      <c r="J89">
+        <v>-118.3086138</v>
+      </c>
     </row>
     <row r="90" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
@@ -10639,6 +10627,12 @@
       <c r="H90" s="3" t="s">
         <v>265</v>
       </c>
+      <c r="I90">
+        <v>34.061946868896399</v>
+      </c>
+      <c r="J90">
+        <v>-118.446640014648</v>
+      </c>
     </row>
     <row r="91" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
@@ -10665,6 +10659,12 @@
       <c r="H91" s="4" t="s">
         <v>384</v>
       </c>
+      <c r="I91">
+        <v>34.044071197509702</v>
+      </c>
+      <c r="J91">
+        <v>-118.71453094482401</v>
+      </c>
     </row>
     <row r="92" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
@@ -10691,6 +10691,12 @@
       <c r="H92" s="3" t="s">
         <v>245</v>
       </c>
+      <c r="I92">
+        <v>34.084932600000002</v>
+      </c>
+      <c r="J92">
+        <v>-118.06774830000001</v>
+      </c>
     </row>
     <row r="93" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
@@ -10717,6 +10723,12 @@
       <c r="H93" s="3" t="s">
         <v>392</v>
       </c>
+      <c r="I93">
+        <v>34.157578999999998</v>
+      </c>
+      <c r="J93">
+        <v>-118.255242</v>
+      </c>
     </row>
     <row r="94" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
@@ -10743,6 +10755,12 @@
       <c r="H94" s="4" t="s">
         <v>397</v>
       </c>
+      <c r="I94">
+        <v>33.810504899999998</v>
+      </c>
+      <c r="J94">
+        <v>-118.134829</v>
+      </c>
     </row>
     <row r="95" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
@@ -10769,6 +10787,12 @@
       <c r="H95" s="3" t="s">
         <v>392</v>
       </c>
+      <c r="I95">
+        <v>33.927337399999999</v>
+      </c>
+      <c r="J95">
+        <v>-118.15884680000001</v>
+      </c>
     </row>
     <row r="96" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
@@ -10795,8 +10819,14 @@
       <c r="H96" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I96">
+        <v>34.041307500000002</v>
+      </c>
+      <c r="J96">
+        <v>-118.12789720000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>47</v>
       </c>
@@ -10821,8 +10851,14 @@
       <c r="H97" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I97">
+        <v>33.831471100000002</v>
+      </c>
+      <c r="J97">
+        <v>-118.30953390000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>47</v>
       </c>
@@ -10847,8 +10883,14 @@
       <c r="H98" s="3" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I98">
+        <v>34.033878199999997</v>
+      </c>
+      <c r="J98">
+        <v>-118.16061759999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>47</v>
       </c>
@@ -10873,19 +10915,25 @@
       <c r="H99" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I99">
+        <v>33.862614299999997</v>
+      </c>
+      <c r="J99">
+        <v>-118.2573742</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="D100" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>417</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>35</v>
@@ -10897,27 +10945,33 @@
         <v>10</v>
       </c>
       <c r="H100" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="I100">
+        <v>33.774382000000003</v>
+      </c>
+      <c r="J100">
+        <v>-118.2762699</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B101" s="4" t="s">
+      <c r="C101" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="D101" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>421</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>12</v>
@@ -10925,19 +10979,25 @@
       <c r="H101" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I101">
+        <v>34.157525999999997</v>
+      </c>
+      <c r="J101">
+        <v>-118.437093</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B102" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="D102" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>20</v>
@@ -10949,21 +11009,27 @@
         <v>10</v>
       </c>
       <c r="H102" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="I102">
+        <v>33.842086399999999</v>
+      </c>
+      <c r="J102">
+        <v>-118.2598924</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B103" s="3" t="s">
+      <c r="C103" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>24</v>
@@ -10977,16 +11043,22 @@
       <c r="H103" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I103">
+        <v>33.915569699999999</v>
+      </c>
+      <c r="J103">
+        <v>-118.07201070000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B104" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>431</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>114</v>
@@ -11003,19 +11075,25 @@
       <c r="H104" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I104" s="1">
+        <v>34.1680055</v>
+      </c>
+      <c r="J104">
+        <v>-118.65976910000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>19</v>
@@ -11029,16 +11107,22 @@
       <c r="H105" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I105" s="1">
+        <v>33.804889000000003</v>
+      </c>
+      <c r="J105">
+        <v>-118.319834</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B106" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>436</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>244</v>
@@ -11047,7 +11131,7 @@
         <v>29</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>12</v>
@@ -11055,45 +11139,57 @@
       <c r="H106" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I106">
+        <v>34.089449000000002</v>
+      </c>
+      <c r="J106">
+        <v>-117.890039</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>42</v>
       </c>
       <c r="H107" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="I107">
+        <v>34.646523199999997</v>
+      </c>
+      <c r="J107">
+        <v>-118.1656541</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B108" s="5" t="s">
+      <c r="C108" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="C108" s="5" t="s">
+      <c r="D108" s="5" t="s">
         <v>444</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>445</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>20</v>
@@ -11105,18 +11201,24 @@
         <v>28</v>
       </c>
       <c r="H108" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="I108">
+        <v>34.075183000000003</v>
+      </c>
+      <c r="J108">
+        <v>-118.039008</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B109" s="5" t="s">
+      <c r="C109" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>241</v>
@@ -11133,19 +11235,25 @@
       <c r="H109" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I109">
+        <v>34.074763300000001</v>
+      </c>
+      <c r="J109">
+        <v>-118.32343710000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C110" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>31</v>
@@ -11159,16 +11267,22 @@
       <c r="H110" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I110">
+        <v>33.915569699999999</v>
+      </c>
+      <c r="J110">
+        <v>-118.07201070000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>451</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>452</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>391</v>
@@ -11185,42 +11299,48 @@
       <c r="H111" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B112" s="3" t="s">
+      <c r="I111" s="3">
+        <v>34.326593299999999</v>
+      </c>
+      <c r="J111">
+        <v>-118.4454272</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="9" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C112" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="D112" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="E112" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F112" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="E112" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F112" s="4" t="s">
+      <c r="G112" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="G112" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B113" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>457</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>458</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>233</v>
@@ -11237,16 +11357,22 @@
       <c r="H113" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I113">
+        <v>34.144410399999998</v>
+      </c>
+      <c r="J113">
+        <v>-118.75499859999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B114" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>412</v>
@@ -11263,19 +11389,25 @@
       <c r="H114" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I114">
+        <v>34.050949699999997</v>
+      </c>
+      <c r="J114">
+        <v>-118.21751</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B115" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="D115" s="6" t="s">
         <v>462</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>463</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>31</v>
@@ -11287,21 +11419,27 @@
         <v>12</v>
       </c>
       <c r="H115" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="I115" s="3">
+        <v>34.040990000000001</v>
+      </c>
+      <c r="J115">
+        <v>-118.25579999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B116" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="3" t="s">
         <v>466</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>467</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -11313,47 +11451,59 @@
         <v>10</v>
       </c>
       <c r="H116" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="I116">
+        <v>34.273451199999997</v>
+      </c>
+      <c r="J116">
+        <v>-118.3392528</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117" s="5" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B117" s="5" t="s">
+      <c r="C117" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="D117" s="4" t="s">
         <v>470</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>471</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H117" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="I117" s="5">
+        <v>34.167380700000002</v>
+      </c>
+      <c r="J117">
+        <v>-118.37749530000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B118" s="3" t="s">
+      <c r="C118" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="D118" s="3" t="s">
         <v>475</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>476</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>19</v>
@@ -11365,21 +11515,27 @@
         <v>10</v>
       </c>
       <c r="H118" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="I118">
+        <v>34.045516967773402</v>
+      </c>
+      <c r="J118">
+        <v>-118.450462341308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B119" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>480</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -11391,21 +11547,27 @@
         <v>10</v>
       </c>
       <c r="H119" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="I119">
+        <v>34.005203999999999</v>
+      </c>
+      <c r="J119">
+        <v>-118.23029699999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B120" s="5" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B120" s="5" t="s">
+      <c r="C120" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="5" t="s">
         <v>483</v>
-      </c>
-      <c r="D120" s="5" t="s">
-        <v>484</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>31</v>
@@ -11414,21 +11576,27 @@
         <v>387</v>
       </c>
       <c r="G120" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="H120" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="H120" s="4" t="s">
+      <c r="I120" s="1">
+        <v>33.991776600000001</v>
+      </c>
+      <c r="J120">
+        <v>-118.0902107</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B121" s="4" t="s">
+      <c r="C121" s="5" t="s">
         <v>487</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>488</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>412</v>
@@ -11440,24 +11608,30 @@
         <v>17</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H121" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I121">
+        <v>33.905442000000001</v>
+      </c>
+      <c r="J121">
+        <v>-118.011612</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B122" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>491</v>
-      </c>
       <c r="D122" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>20</v>
@@ -11471,16 +11645,22 @@
       <c r="H122" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I122">
+        <v>33.927031700000001</v>
+      </c>
+      <c r="J122">
+        <v>-118.19968179999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>233</v>
@@ -11497,19 +11677,25 @@
       <c r="H123" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I123">
+        <v>34.1394844055175</v>
+      </c>
+      <c r="J123">
+        <v>-118.679809570312</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B124" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>495</v>
-      </c>
       <c r="D124" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>20</v>
@@ -11518,21 +11704,27 @@
         <v>387</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I124">
+        <v>34.012130737304602</v>
+      </c>
+      <c r="J124">
+        <v>-118.117752075195</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>351</v>
@@ -11547,21 +11739,27 @@
         <v>10</v>
       </c>
       <c r="H125" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="I125">
+        <v>34.417878299999998</v>
+      </c>
+      <c r="J125">
+        <v>-118.4549835</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B126" s="1" t="s">
+      <c r="C126" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="D126" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>502</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>20</v>
@@ -11575,16 +11773,22 @@
       <c r="H126" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I126">
+        <v>34.065201799999997</v>
+      </c>
+      <c r="J126">
+        <v>-118.2349652</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B127" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>504</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>96</v>
@@ -11593,79 +11797,97 @@
         <v>31</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H127" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="I127">
+        <v>34.142956099999999</v>
+      </c>
+      <c r="J127">
+        <v>-117.977447</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A128" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B128" s="3" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B128" s="3" t="s">
+      <c r="C128" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>509</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H128" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="I128">
+        <v>34.612114900000002</v>
+      </c>
+      <c r="J128">
+        <v>-117.8256935</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B129" s="4" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B129" s="4" t="s">
+      <c r="C129" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="D129" s="4" t="s">
         <v>513</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>514</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H129" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I129">
+        <v>34.025760099999999</v>
+      </c>
+      <c r="J129">
+        <v>-118.2750656</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B130" s="3" t="s">
+      <c r="C130" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="D130" s="3" t="s">
         <v>518</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>519</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>20</v>
@@ -11679,19 +11901,25 @@
       <c r="H130" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I130" s="5">
+        <v>34.176891326904297</v>
+      </c>
+      <c r="J130">
+        <v>-118.589630126953</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B131" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>522</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -11703,18 +11931,24 @@
         <v>10</v>
       </c>
       <c r="H131" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="I131" s="1">
+        <v>33.903591156005803</v>
+      </c>
+      <c r="J131">
+        <v>-118.16022491455</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A132" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B132" s="1" t="s">
+      <c r="C132" s="3" t="s">
         <v>524</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>525</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>77</v>
@@ -11731,16 +11965,22 @@
       <c r="H132" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I132" s="3">
+        <v>34.046120700000003</v>
+      </c>
+      <c r="J132">
+        <v>-118.04683540000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B133" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>527</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>54</v>
@@ -11757,19 +11997,25 @@
       <c r="H133" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I133">
+        <v>33.884380499999999</v>
+      </c>
+      <c r="J133">
+        <v>-118.12382719999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B134" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>530</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>19</v>
@@ -11781,21 +12027,27 @@
         <v>10</v>
       </c>
       <c r="H134" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="I134">
+        <v>34.029247300000002</v>
+      </c>
+      <c r="J134">
+        <v>-118.41236069999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A135" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B135" s="3" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B135" s="3" t="s">
+      <c r="C135" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="C135" s="3" t="s">
+      <c r="D135" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>534</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -11807,18 +12059,24 @@
         <v>10</v>
       </c>
       <c r="H135" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I135" s="3">
+        <v>34.172862500000001</v>
+      </c>
+      <c r="J135">
+        <v>-118.614487</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A136" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B136" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>408</v>
@@ -11830,24 +12088,30 @@
         <v>21</v>
       </c>
       <c r="G136" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="H136" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="H136" s="3" t="s">
+      <c r="I136">
+        <v>34.066494900000002</v>
+      </c>
+      <c r="J136">
+        <v>-118.1671415</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A137" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B137" s="1" t="s">
+      <c r="C137" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C137" s="3" t="s">
-        <v>541</v>
-      </c>
       <c r="D137" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>24</v>
@@ -11859,73 +12123,85 @@
         <v>10</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>522</v>
+      </c>
+      <c r="I137">
+        <v>33.861419599999998</v>
+      </c>
+      <c r="J137">
+        <v>-118.2806935</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B138" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="C138" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="D138" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="D138" s="5" t="s">
-        <v>544</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G138" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H138" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="I138">
+        <v>34.032677100000001</v>
+      </c>
+      <c r="J138">
+        <v>-118.2923761</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A139" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B139" s="8" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B139" s="1" t="s">
+      <c r="C139" s="7" t="s">
         <v>547</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="D139" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="E139" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F139" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G139" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A140" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B140" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="E139" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H139" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B140" s="3" t="s">
+      <c r="C140" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>551</v>
-      </c>
       <c r="D140" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>29</v>
@@ -11937,18 +12213,24 @@
         <v>10</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>522</v>
+      </c>
+      <c r="I140" s="1">
+        <v>33.968491100000001</v>
+      </c>
+      <c r="J140">
+        <v>-118.14393939999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B141" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>552</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>553</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>391</v>
@@ -11965,16 +12247,22 @@
       <c r="H141" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I141">
+        <v>34.059405599999998</v>
+      </c>
+      <c r="J141">
+        <v>-118.20923759999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>554</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>555</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>233</v>
@@ -11986,21 +12274,27 @@
         <v>25</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I142">
+        <v>33.783954000000001</v>
+      </c>
+      <c r="J142">
+        <v>-118.108103</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B143" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>558</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>233</v>
@@ -12017,16 +12311,22 @@
       <c r="H143" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I143" s="3">
+        <v>34.216630100000003</v>
+      </c>
+      <c r="J143">
+        <v>-118.5361717</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B144" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>559</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>560</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>233</v>
@@ -12041,18 +12341,24 @@
         <v>10</v>
       </c>
       <c r="H144" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="I144">
+        <v>34.173377100000003</v>
+      </c>
+      <c r="J144">
+        <v>-118.5939293</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B145" s="4" t="s">
+      <c r="C145" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="C145" s="5" t="s">
-        <v>563</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>395</v>
@@ -12069,45 +12375,57 @@
       <c r="H145" s="4" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I145" s="5">
+        <v>33.848620099999998</v>
+      </c>
+      <c r="J145">
+        <v>-118.1336726</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B146" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="D146" s="3" t="s">
         <v>565</v>
-      </c>
-      <c r="D146" s="3" t="s">
-        <v>566</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H146" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="I146" s="3">
+        <v>34.199706300000003</v>
+      </c>
+      <c r="J146">
+        <v>-118.62988060000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B147" s="4" t="s">
+      <c r="C147" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="D147" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>571</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>31</v>
@@ -12121,45 +12439,57 @@
       <c r="H147" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I147">
+        <v>33.877596199999999</v>
+      </c>
+      <c r="J147">
+        <v>-118.2114607</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B148" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C148" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>574</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H148" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="I148">
+        <v>34.004147000000003</v>
+      </c>
+      <c r="J148">
+        <v>-118.3308304</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A149" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B149" s="3" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B149" s="3" t="s">
+      <c r="C149" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="C149" s="3" t="s">
-        <v>578</v>
-      </c>
       <c r="D149" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>24</v>
@@ -12168,10 +12498,16 @@
         <v>300</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
+      </c>
+      <c r="I149">
+        <v>33.978806499999997</v>
+      </c>
+      <c r="J149">
+        <v>-118.032297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced null variables with 1000 so I can filter out later
</commit_message>
<xml_diff>
--- a/CurrentMrktsCounty.xlsx
+++ b/CurrentMrktsCounty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chesneymelissinos/Desktop/Coding/lafpc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706AC4C0-B089-844E-B3B6-0EE524CAAA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5E8E57-F974-114A-8590-F29219553D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="500" windowWidth="26480" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7864,7 +7864,7 @@
   <dimension ref="A1:J149"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="I149" sqref="I149"/>
+      <selection activeCell="I158" sqref="I158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7935,6 +7935,12 @@
       <c r="H2" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="I2" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -7961,6 +7967,12 @@
       <c r="H3" s="10" t="s">
         <v>57</v>
       </c>
+      <c r="I3" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -8147,6 +8159,12 @@
       <c r="H9" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="I9" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
@@ -8173,6 +8191,12 @@
       <c r="H10" s="7" t="s">
         <v>86</v>
       </c>
+      <c r="I10" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
@@ -8197,6 +8221,12 @@
         <v>12</v>
       </c>
       <c r="H11" s="8"/>
+      <c r="I11" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J11" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
@@ -8543,6 +8573,12 @@
       <c r="H22" s="7" t="s">
         <v>137</v>
       </c>
+      <c r="I22" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="23" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
@@ -8569,6 +8605,12 @@
       <c r="H23" s="7" t="s">
         <v>141</v>
       </c>
+      <c r="I23" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
@@ -8691,6 +8733,12 @@
       <c r="H27" s="10" t="s">
         <v>157</v>
       </c>
+      <c r="I27" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J27" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
@@ -8909,6 +8957,12 @@
       <c r="H34" s="7" t="s">
         <v>184</v>
       </c>
+      <c r="I34" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J34" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
@@ -8997,6 +9051,12 @@
         <v>10</v>
       </c>
       <c r="H37" s="12"/>
+      <c r="I37" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J37" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
@@ -9023,6 +9083,12 @@
       <c r="H38" s="10" t="s">
         <v>115</v>
       </c>
+      <c r="I38" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J38" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
@@ -9145,6 +9211,12 @@
       <c r="H42" s="10" t="s">
         <v>211</v>
       </c>
+      <c r="I42" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J42" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="43" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
@@ -9235,6 +9307,12 @@
       <c r="H45" s="10" t="s">
         <v>223</v>
       </c>
+      <c r="I45" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J45" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="46" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
@@ -9261,6 +9339,12 @@
       <c r="H46" s="7" t="s">
         <v>227</v>
       </c>
+      <c r="I46" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J46" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
@@ -9863,6 +9947,12 @@
       <c r="H65" s="7" t="s">
         <v>296</v>
       </c>
+      <c r="I65" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J65" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="66" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
@@ -10017,6 +10107,12 @@
       <c r="H70" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="I70" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J70" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="71" spans="1:10" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
@@ -10043,6 +10139,12 @@
       <c r="H71" s="10" t="s">
         <v>317</v>
       </c>
+      <c r="I71" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J71" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="72" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
@@ -10421,6 +10523,12 @@
       <c r="H83" s="7" t="s">
         <v>353</v>
       </c>
+      <c r="I83" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J83" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="84" spans="1:10" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="7" t="s">
@@ -10447,6 +10555,12 @@
       <c r="H84" s="7" t="s">
         <v>358</v>
       </c>
+      <c r="I84" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J84" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="85" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
@@ -10537,6 +10651,12 @@
       <c r="H87" s="7" t="s">
         <v>368</v>
       </c>
+      <c r="I87" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J87" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="88" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
@@ -11331,6 +11451,12 @@
       <c r="H112" s="10" t="s">
         <v>115</v>
       </c>
+      <c r="I112" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J112" s="9">
+        <v>1000</v>
+      </c>
     </row>
     <row r="113" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
@@ -12188,6 +12314,12 @@
       </c>
       <c r="H139" s="7" t="s">
         <v>522</v>
+      </c>
+      <c r="I139" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J139" s="9">
+        <v>1000</v>
       </c>
     </row>
     <row r="140" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>